<commit_message>
training with new data
</commit_message>
<xml_diff>
--- a/data/seizure_metadata.xlsx
+++ b/data/seizure_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kikal\OneDrive\Documentos\WorkspaceCarolina\AIB\Module2\Aitana\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C820F3FE-BA51-4898-8A99-510CF5225705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4E3497-DD6D-4400-A35F-238257A3B863}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" activeTab="2" xr2:uid="{69F3FABD-DFB9-4A6F-9630-8A75EF3ECECA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{69F3FABD-DFB9-4A6F-9630-8A75EF3ECECA}"/>
   </bookViews>
   <sheets>
     <sheet name="disk" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="90">
   <si>
     <t>id,class,clinical_begin,clinical_end</t>
   </si>
@@ -281,9 +281,6 @@
   </si>
   <si>
     <t>Time</t>
-  </si>
-  <si>
-    <t>Test (1) or Train (0)?</t>
   </si>
   <si>
     <t>456.66</t>
@@ -1058,10 +1055,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9829353B-5420-4673-91E7-388CDDF52CB8}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="72" zoomScaleNormal="72" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="M1" sqref="M1:M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1079,7 +1076,7 @@
     <col min="12" max="12" width="11.81640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="4" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="66" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>31</v>
       </c>
@@ -1116,11 +1113,8 @@
       <c r="L1" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>32</v>
       </c>
@@ -1159,11 +1153,8 @@
       <c r="L2" s="3">
         <v>1</v>
       </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1202,11 +1193,8 @@
       <c r="L3" s="3">
         <v>0</v>
       </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>32</v>
       </c>
@@ -1245,11 +1233,8 @@
       <c r="L4" s="3">
         <v>0</v>
       </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1288,11 +1273,8 @@
       <c r="L5" s="3">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -1331,11 +1313,8 @@
       <c r="L6" s="3">
         <v>1</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1374,11 +1353,8 @@
       <c r="L7" s="3">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1417,11 +1393,8 @@
       <c r="L8" s="3">
         <v>1</v>
       </c>
-      <c r="M8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>32</v>
       </c>
@@ -1460,11 +1433,8 @@
       <c r="L9" s="3">
         <v>1</v>
       </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1503,11 +1473,8 @@
       <c r="L10" s="3">
         <v>1</v>
       </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>33</v>
       </c>
@@ -1532,7 +1499,7 @@
         <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I11" t="s">
         <v>73</v>
@@ -1546,11 +1513,8 @@
       <c r="L11" s="3">
         <v>1</v>
       </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1575,7 +1539,7 @@
         <v>46</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
         <v>73</v>
@@ -1589,11 +1553,8 @@
       <c r="L12" s="3">
         <v>0</v>
       </c>
-      <c r="M12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1618,7 +1579,7 @@
         <v>47</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I13" t="s">
         <v>73</v>
@@ -1632,11 +1593,8 @@
       <c r="L13" s="3">
         <v>0</v>
       </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -1661,7 +1619,7 @@
         <v>48</v>
       </c>
       <c r="H14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I14" t="s">
         <v>73</v>
@@ -1675,11 +1633,8 @@
       <c r="L14" s="3">
         <v>1</v>
       </c>
-      <c r="M14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -1704,7 +1659,7 @@
         <v>49</v>
       </c>
       <c r="H15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="I15" t="s">
         <v>73</v>
@@ -1718,11 +1673,8 @@
       <c r="L15" s="3">
         <v>1</v>
       </c>
-      <c r="M15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1747,7 +1699,7 @@
         <v>50</v>
       </c>
       <c r="H16" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I16" t="s">
         <v>73</v>
@@ -1761,11 +1713,8 @@
       <c r="L16" s="3">
         <v>1</v>
       </c>
-      <c r="M16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1790,7 +1739,7 @@
         <v>51</v>
       </c>
       <c r="H17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I17" t="s">
         <v>73</v>
@@ -1804,11 +1753,8 @@
       <c r="L17" s="3">
         <v>1</v>
       </c>
-      <c r="M17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>33</v>
       </c>
@@ -1833,7 +1779,7 @@
         <v>52</v>
       </c>
       <c r="H18" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I18" t="s">
         <v>73</v>
@@ -1847,11 +1793,8 @@
       <c r="L18" s="3">
         <v>0</v>
       </c>
-      <c r="M18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -1876,7 +1819,7 @@
         <v>53</v>
       </c>
       <c r="H19" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I19" t="s">
         <v>73</v>
@@ -1889,9 +1832,6 @@
       </c>
       <c r="L19" s="3">
         <v>0</v>
-      </c>
-      <c r="M19">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>